<commit_message>
fixed template link, template format, file upload worker, added loading gif to audit view, added indexes to Sample fields
</commit_message>
<xml_diff>
--- a/sampledbapp/static/xls_templates/template1.xlsx
+++ b/sampledbapp/static/xls_templates/template1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16600" windowHeight="8280"/>
+    <workbookView xWindow="3340" yWindow="460" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample List" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,75 +21,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Parent Type</t>
-  </si>
-  <si>
-    <t>Parent ID</t>
-  </si>
-  <si>
-    <t>Consent Form Information</t>
-  </si>
-  <si>
-    <t>Tissue Bank Collection</t>
-  </si>
-  <si>
-    <t>Hazard Group</t>
-  </si>
-  <si>
-    <t>Hazard Description</t>
-  </si>
-  <si>
-    <t>Storage Type</t>
-  </si>
-  <si>
-    <t>Campus</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Freezer</t>
-  </si>
-  <si>
-    <t>Shelf Name</t>
-  </si>
-  <si>
-    <t>Shelf Barcode</t>
-  </si>
-  <si>
-    <t>Box Name</t>
-  </si>
-  <si>
-    <t>Box Barcode</t>
-  </si>
-  <si>
-    <t>Type</t>
+    <t>study_title</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>sample_storage_type</t>
+  </si>
+  <si>
+    <t>sample_matrix</t>
+  </si>
+  <si>
+    <t>collection_protocol</t>
+  </si>
+  <si>
+    <t>campus</t>
+  </si>
+  <si>
+    <t>building</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>freezer_id</t>
+  </si>
+  <si>
+    <t>shelf_id</t>
+  </si>
+  <si>
+    <t>box_id</t>
+  </si>
+  <si>
+    <t>parent_type</t>
+  </si>
+  <si>
+    <t>parent_id</t>
+  </si>
+  <si>
+    <t>consent_form_information</t>
+  </si>
+  <si>
+    <t>tissue_bank_reference</t>
+  </si>
+  <si>
+    <t>hazard_group</t>
+  </si>
+  <si>
+    <t>hazard_description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,23 +108,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -281,20 +264,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -416,93 +395,118 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixed the commit new samples worker
</commit_message>
<xml_diff>
--- a/sampledbapp/static/xls_templates/template1.xlsx
+++ b/sampledbapp/static/xls_templates/template1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>study_title</t>
   </si>
@@ -73,6 +73,57 @@
   </si>
   <si>
     <t>hazard_description</t>
+  </si>
+  <si>
+    <t>study title test1</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>SAF</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>45678</t>
+  </si>
+  <si>
+    <t>human id</t>
+  </si>
+  <si>
+    <t>human1</t>
+  </si>
+  <si>
+    <t>Consent form is here...</t>
+  </si>
+  <si>
+    <t>THIS-IS-A-CODE</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>G134</t>
+  </si>
+  <si>
+    <t>Eppendorf</t>
   </si>
 </sst>
 </file>
@@ -441,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -505,6 +556,62 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
fixed template file, project title order, and width of pending commit widgets
</commit_message>
<xml_diff>
--- a/sampledbapp/static/xls_templates/template1.xlsx
+++ b/sampledbapp/static/xls_templates/template1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="460" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="1640" windowWidth="25040" windowHeight="14420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="My Samples" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="52">
   <si>
     <t>study_title</t>
   </si>
@@ -75,65 +75,132 @@
     <t>hazard_description</t>
   </si>
   <si>
-    <t>study title test1</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
     <t>Human</t>
   </si>
   <si>
-    <t>Plasma</t>
-  </si>
-  <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>SAF</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>45678</t>
-  </si>
-  <si>
-    <t>human id</t>
-  </si>
-  <si>
-    <t>human1</t>
-  </si>
-  <si>
-    <t>Consent form is here...</t>
-  </si>
-  <si>
-    <t>THIS-IS-A-CODE</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>G134</t>
-  </si>
-  <si>
-    <t>Eppendorf</t>
+    <t>eppendorf tube</t>
+  </si>
+  <si>
+    <t>Urine</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>My REC Code</t>
+  </si>
+  <si>
+    <t>My box code</t>
+  </si>
+  <si>
+    <t>Filtered</t>
+  </si>
+  <si>
+    <t>My tissue bank ref</t>
+  </si>
+  <si>
+    <t>human origin - filtered</t>
+  </si>
+  <si>
+    <t>My new study 1</t>
+  </si>
+  <si>
+    <t>Sample 1</t>
+  </si>
+  <si>
+    <t>Sample 2</t>
+  </si>
+  <si>
+    <t>Sample 3</t>
+  </si>
+  <si>
+    <t>Sample 4</t>
+  </si>
+  <si>
+    <t>Sample 5</t>
+  </si>
+  <si>
+    <t>Sample 6</t>
+  </si>
+  <si>
+    <t>Sample 7</t>
+  </si>
+  <si>
+    <t>Sample 8</t>
+  </si>
+  <si>
+    <t>Sample 9</t>
+  </si>
+  <si>
+    <t>Sample 10</t>
+  </si>
+  <si>
+    <t>Room Number</t>
+  </si>
+  <si>
+    <t>Freezer 4</t>
+  </si>
+  <si>
+    <t>Patient 1</t>
+  </si>
+  <si>
+    <t>Patient 2</t>
+  </si>
+  <si>
+    <t>Patient 3</t>
+  </si>
+  <si>
+    <t>Patient 4</t>
+  </si>
+  <si>
+    <t>Patient 5</t>
+  </si>
+  <si>
+    <t>Patient 6</t>
+  </si>
+  <si>
+    <t>Patient 7</t>
+  </si>
+  <si>
+    <t>Patient 8</t>
+  </si>
+  <si>
+    <t>Patient 9</t>
+  </si>
+  <si>
+    <t>Patient 10</t>
+  </si>
+  <si>
+    <t>building name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,17 +223,81 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="33">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -245,7 +376,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -280,7 +410,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -315,16 +444,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -446,59 +579,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -558,62 +661,567 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="N7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>